<commit_message>
rename tab in submission spreadsheet from DesireEditedSequences to TargetedSearch, output config name amplicount_sequences.csv to amplicount_config_tsearch.csv, output result name amplicount_desired_edits.csv to amplicount_tsearch.csv, and column name desired_seq_id to tsearch_id
</commit_message>
<xml_diff>
--- a/data/sra_metadata/SRP198941_SLX15021_GEP00005.xlsx
+++ b/data/sra_metadata/SRP198941_SLX15021_GEP00005.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="736" activeTab="1"/>
+    <workbookView xWindow="2460" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="736"/>
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="13" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="Layout" sheetId="6" r:id="rId5"/>
     <sheet name="Plate" sheetId="7" r:id="rId6"/>
     <sheet name="GuideMismatches" sheetId="4" r:id="rId7"/>
-    <sheet name="DesireEditedSequences" sheetId="12" r:id="rId8"/>
+    <sheet name="TargetedSearch" sheetId="12" r:id="rId8"/>
     <sheet name="Menus" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
@@ -1982,6 +1982,26 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">This name must match </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Guide@name</t>
+    </r>
+  </si>
+  <si>
+    <t>amplicon_name</t>
+  </si>
+  <si>
+    <t>TargetedSearch</t>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">The </t>
     </r>
     <r>
@@ -1991,7 +2011,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>DesireEditedSequences</t>
+      <t>TargetedSearch</t>
     </r>
     <r>
       <rPr>
@@ -2001,26 +2021,6 @@
       </rPr>
       <t xml:space="preserve"> is the list of sequence to count the reads against. If not provided, all sequences above a certain threshold will be considered for counting the reads.   </t>
     </r>
-  </si>
-  <si>
-    <t>DesireEditedSequences</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">This name must match </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Guide@name</t>
-    </r>
-  </si>
-  <si>
-    <t>amplicon_name</t>
   </si>
 </sst>
 </file>
@@ -2450,6 +2450,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2459,7 +2460,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="191">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2657,19 +2657,6 @@
   <dxfs count="132">
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2806,6 +2793,170 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2823,6 +2974,74 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -2840,111 +3059,182 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -3042,6 +3332,23 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -3059,6 +3366,40 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -3077,347 +3418,6 @@
     <dxf>
       <font>
         <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -4931,59 +4931,59 @@
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="42" name="Table42" displayName="Table42" ref="A1:N9" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
   <tableColumns count="14">
-    <tableColumn id="14" name="amplicon_name" dataDxfId="1"/>
-    <tableColumn id="1" name="guide_name" dataDxfId="60"/>
-    <tableColumn id="2" name="experiment_type" dataDxfId="59"/>
-    <tableColumn id="3" name="guide_location" dataDxfId="58"/>
-    <tableColumn id="4" name="guide_strand" dataDxfId="57"/>
-    <tableColumn id="5" name="is_on_target" dataDxfId="56"/>
-    <tableColumn id="6" name="dna_feature" dataDxfId="55"/>
-    <tableColumn id="7" name="chrom" dataDxfId="54"/>
-    <tableColumn id="8" name="forward_primer_sequence" dataDxfId="53"/>
-    <tableColumn id="9" name="forward_primer_start" dataDxfId="52"/>
-    <tableColumn id="10" name="forward_primer_end" dataDxfId="51"/>
-    <tableColumn id="11" name="reverse_primer_sequence" dataDxfId="50"/>
-    <tableColumn id="12" name="reverse_primer_start" dataDxfId="49"/>
-    <tableColumn id="13" name="reverse_primer_end" dataDxfId="48"/>
+    <tableColumn id="14" name="amplicon_name" dataDxfId="60"/>
+    <tableColumn id="1" name="guide_name" dataDxfId="59"/>
+    <tableColumn id="2" name="experiment_type" dataDxfId="58"/>
+    <tableColumn id="3" name="guide_location" dataDxfId="57"/>
+    <tableColumn id="4" name="guide_strand" dataDxfId="56"/>
+    <tableColumn id="5" name="is_on_target" dataDxfId="55"/>
+    <tableColumn id="6" name="dna_feature" dataDxfId="54"/>
+    <tableColumn id="7" name="chrom" dataDxfId="53"/>
+    <tableColumn id="8" name="forward_primer_sequence" dataDxfId="52"/>
+    <tableColumn id="9" name="forward_primer_start" dataDxfId="51"/>
+    <tableColumn id="10" name="forward_primer_end" dataDxfId="50"/>
+    <tableColumn id="11" name="reverse_primer_sequence" dataDxfId="49"/>
+    <tableColumn id="12" name="reverse_primer_start" dataDxfId="48"/>
+    <tableColumn id="13" name="reverse_primer_end" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="43" name="Table43" displayName="Table43" ref="O1:P9" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="43" name="Table43" displayName="Table43" ref="O1:P9" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
   <tableColumns count="2">
-    <tableColumn id="1" name="score" dataDxfId="45"/>
-    <tableColumn id="2" name="description" dataDxfId="44"/>
+    <tableColumn id="1" name="score" dataDxfId="44"/>
+    <tableColumn id="2" name="description" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="44" name="Table44" displayName="Table44" ref="A1:C475" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="44" name="Table44" displayName="Table44" ref="A1:C475" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <tableColumns count="3">
-    <tableColumn id="1" name="layout_id" dataDxfId="41"/>
-    <tableColumn id="2" name="well_position" dataDxfId="40"/>
-    <tableColumn id="13" name="sequencing_barcode" dataDxfId="39"/>
+    <tableColumn id="1" name="layout_id" dataDxfId="40"/>
+    <tableColumn id="2" name="well_position" dataDxfId="39"/>
+    <tableColumn id="13" name="sequencing_barcode" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="46" name="Table46" displayName="Table46" ref="D1:M475" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="46" name="Table46" displayName="Table46" ref="D1:M475" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
   <tableColumns count="10">
-    <tableColumn id="1" name="sequencing_sample_name" dataDxfId="36"/>
-    <tableColumn id="2" name="sequencing_dna_source" dataDxfId="35"/>
-    <tableColumn id="3" name="sequencing_library_type" dataDxfId="34"/>
-    <tableColumn id="4" name="sequencing_project_id" dataDxfId="33"/>
-    <tableColumn id="5" name="cell_line_name" dataDxfId="32"/>
-    <tableColumn id="6" name="cell_pool" dataDxfId="31"/>
-    <tableColumn id="7" name="clone_name" dataDxfId="30"/>
-    <tableColumn id="8" name="content_type" dataDxfId="29"/>
-    <tableColumn id="9" name="is_control" dataDxfId="28"/>
-    <tableColumn id="10" name="replicate_group" dataDxfId="27"/>
+    <tableColumn id="1" name="sequencing_sample_name" dataDxfId="35"/>
+    <tableColumn id="2" name="sequencing_dna_source" dataDxfId="34"/>
+    <tableColumn id="3" name="sequencing_library_type" dataDxfId="33"/>
+    <tableColumn id="4" name="sequencing_project_id" dataDxfId="32"/>
+    <tableColumn id="5" name="cell_line_name" dataDxfId="31"/>
+    <tableColumn id="6" name="cell_pool" dataDxfId="30"/>
+    <tableColumn id="7" name="clone_name" dataDxfId="29"/>
+    <tableColumn id="8" name="content_type" dataDxfId="28"/>
+    <tableColumn id="9" name="is_control" dataDxfId="27"/>
+    <tableColumn id="10" name="replicate_group" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5001,50 +5001,50 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="51" name="Table51" displayName="Table51" ref="A1:D10" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="51" name="Table51" displayName="Table51" ref="A1:D10" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <tableColumns count="4">
-    <tableColumn id="1" name="layout_id" dataDxfId="24"/>
-    <tableColumn id="2" name="plate_name" dataDxfId="23"/>
-    <tableColumn id="5" name="plate_barcode" dataDxfId="22"/>
-    <tableColumn id="4" name="plate_description" dataDxfId="21"/>
+    <tableColumn id="1" name="layout_id" dataDxfId="23"/>
+    <tableColumn id="2" name="plate_name" dataDxfId="22"/>
+    <tableColumn id="5" name="plate_barcode" dataDxfId="21"/>
+    <tableColumn id="4" name="plate_description" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table18" displayName="Table18" ref="A1:D31" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table18" displayName="Table18" ref="A1:D31" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <tableColumns count="4">
-    <tableColumn id="1" name="guide_name" dataDxfId="18"/>
-    <tableColumn id="2" name="is_off_target_coding_region" dataDxfId="17"/>
-    <tableColumn id="3" name="number_of_mismatches" dataDxfId="16"/>
-    <tableColumn id="4" name="number_of_off_targets" dataDxfId="15"/>
+    <tableColumn id="1" name="guide_name" dataDxfId="17"/>
+    <tableColumn id="2" name="is_off_target_coding_region" dataDxfId="16"/>
+    <tableColumn id="3" name="number_of_mismatches" dataDxfId="15"/>
+    <tableColumn id="4" name="number_of_off_targets" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table1141" displayName="Table1141" ref="A1:C9" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table1141" displayName="Table1141" ref="A1:C9" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="3">
-    <tableColumn id="3" name="amplicon_name" dataDxfId="0" dataCellStyle="Normal"/>
-    <tableColumn id="1" name="sequence_name" dataDxfId="12" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="sequence" dataDxfId="11" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="amplicon_name" dataDxfId="11" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="sequence_name" dataDxfId="10" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="sequence" dataDxfId="9" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G9" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G9" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <tableColumns count="7">
-    <tableColumn id="1" name="target_genome" dataDxfId="8"/>
-    <tableColumn id="2" name="strand" dataDxfId="7"/>
-    <tableColumn id="3" name="dna_feature" dataDxfId="6"/>
-    <tableColumn id="4" name="is_true_or_false" dataDxfId="5"/>
-    <tableColumn id="5" name="cell_line_name" dataDxfId="4"/>
-    <tableColumn id="6" name="content_type" dataDxfId="3"/>
-    <tableColumn id="7" name="sequencing_dna_source" dataDxfId="2"/>
+    <tableColumn id="1" name="target_genome" dataDxfId="6"/>
+    <tableColumn id="2" name="strand" dataDxfId="5"/>
+    <tableColumn id="3" name="dna_feature" dataDxfId="4"/>
+    <tableColumn id="4" name="is_true_or_false" dataDxfId="3"/>
+    <tableColumn id="5" name="cell_line_name" dataDxfId="2"/>
+    <tableColumn id="6" name="content_type" dataDxfId="1"/>
+    <tableColumn id="7" name="sequencing_dna_source" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5454,7 +5454,7 @@
   </sheetPr>
   <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
@@ -5467,25 +5467,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="32">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>244</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
     </row>
     <row r="2" spans="1:3" ht="20">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="27" t="s">
         <v>245</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
     </row>
     <row r="3" spans="1:3" ht="18">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="28" t="s">
         <v>242</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
@@ -6021,7 +6021,7 @@
         <v>4</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -6061,10 +6061,10 @@
     </row>
     <row r="74" spans="1:3" ht="30">
       <c r="A74" s="1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -6120,7 +6120,7 @@
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -6527,7 +6527,7 @@
   <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6554,7 +6554,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>4</v>
@@ -6968,7 +6968,7 @@
   <dimension ref="A1:M97"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11420,8 +11420,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15">
-      <c r="A1" s="28" t="s">
-        <v>498</v>
+      <c r="A1" s="25" t="s">
+        <v>496</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>492</v>
@@ -11431,42 +11431,42 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15">
-      <c r="A2" s="28"/>
+      <c r="A2" s="25"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" ht="15">
-      <c r="A3" s="28"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" ht="15">
-      <c r="A4" s="28"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" ht="15">
-      <c r="A5" s="28"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" ht="15">
-      <c r="A6" s="28"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" ht="15">
-      <c r="A7" s="28"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" ht="15">
-      <c r="A8" s="28"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" ht="15">
-      <c r="A9" s="28"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>

</xml_diff>

<commit_message>
update doc on submission spreadsheet for TargetedSearch
</commit_message>
<xml_diff>
--- a/data/sra_metadata/SRP198941_SLX15021_GEP00005.xlsx
+++ b/data/sra_metadata/SRP198941_SLX15021_GEP00005.xlsx
@@ -2019,7 +2019,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> is the list of sequence to count the reads against. If not provided, all sequences above a certain threshold will be considered for counting the reads.   </t>
+      <t xml:space="preserve"> is a list of sequences that the reads are counted against. If looking for particular gene edits, the desired edited sequences should be put in here. If no sequence is provided, the amplicon as identified by the provided primer sequences will be considered for counting reads</t>
     </r>
   </si>
 </sst>
@@ -6059,7 +6059,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="30">
+    <row r="74" spans="1:3" ht="45">
       <c r="A74" s="1" t="s">
         <v>497</v>
       </c>

</xml_diff>